<commit_message>
Idk, most likely delete
</commit_message>
<xml_diff>
--- a/Bili.xlsx
+++ b/Bili.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\plocha\lovv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\plocha\Billionaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21832FB6-CFB7-4E00-A15E-43B3C0C9C36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03463F3E-0655-4024-B412-AC93788E62C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5551,8 +5551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0994256-6C2A-4050-AD0D-ACCB33202366}">
   <dimension ref="A1:L238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>